<commit_message>
[Hai: new] Complete testcase verion 1.0
</commit_message>
<xml_diff>
--- a/Testcase/Version 1.0/Group03_Testcase_Ver1.0.xlsx
+++ b/Testcase/Version 1.0/Group03_Testcase_Ver1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Refferences\HK2_2020_2021\Software_Engineering\FinalProject\AppTangQua\Testcase\Version 1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F37CC7-BFD3-4E99-BB7F-039A8A8BB5B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6398A1F-02AB-4868-A536-4CCD3206FFFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1693A64A-044D-4DAF-8A90-D04091905ADA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="6" xr2:uid="{1693A64A-044D-4DAF-8A90-D04091905ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TC_004" sheetId="4" r:id="rId4"/>
     <sheet name="TC_005" sheetId="5" r:id="rId5"/>
     <sheet name="TC_006" sheetId="6" r:id="rId6"/>
+    <sheet name="TC_007" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="83">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -222,6 +223,63 @@
   </si>
   <si>
     <t>Cutomer receive an error annouce</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>Test the AddProduct Functionality in GiftsApp</t>
+  </si>
+  <si>
+    <t>Đức</t>
+  </si>
+  <si>
+    <t>Have account with role as Admin</t>
+  </si>
+  <si>
+    <t>ImageURL (String)</t>
+  </si>
+  <si>
+    <t>Access to from AddProduct</t>
+  </si>
+  <si>
+    <t>ProductName = Gấu bông (String)</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Object = Nam/Nữ/Bé/Nam&amp;Nữ (String)</t>
+  </si>
+  <si>
+    <t>Occasion = Sinh nhật/Tân gia (String)</t>
+  </si>
+  <si>
+    <t>Holiday = valentine/(8/3)/Giáng Sinh (String)</t>
+  </si>
+  <si>
+    <t>Description = Gấu bông cho bé (String)</t>
+  </si>
+  <si>
+    <t>Product Quantity  = 2 (Number)</t>
+  </si>
+  <si>
+    <t>Product Price = 200000 (String)</t>
+  </si>
+  <si>
+    <t>Write requie field in form AddProduct and click Thêm this Object (Product) will be store on firebase</t>
+  </si>
+  <si>
+    <t>Write all field on form AddProduct</t>
+  </si>
+  <si>
+    <t>Can bi write</t>
+  </si>
+  <si>
+    <t>Object (Product) can be storage on firebase</t>
+  </si>
+  <si>
+    <t>Click "Thêm"</t>
   </si>
 </sst>
 </file>
@@ -370,7 +428,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -414,6 +472,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -424,71 +511,63 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,55 +886,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C369C98-2EF7-44D9-AD66-D4670DC9D9A1}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -871,10 +950,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -899,29 +978,29 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38">
+      <c r="E6" s="22"/>
+      <c r="F6" s="42">
         <v>44322</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="23" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -940,94 +1019,94 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="2"/>
       <c r="F9" s="10">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="2"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="2"/>
       <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="2"/>
       <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1060,122 +1139,122 @@
       <c r="K14" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
     </row>
     <row r="42" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1186,41 +1265,6 @@
     <row r="130" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="D16:E17"/>
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G8:K8"/>
@@ -1231,6 +1275,41 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="G12:K12"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1247,48 +1326,48 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
@@ -1304,10 +1383,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1332,29 +1411,29 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38">
+      <c r="E6" s="22"/>
+      <c r="F6" s="42">
         <v>44322</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="23" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1373,94 +1452,94 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14"/>
       <c r="F9" s="10">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="14"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="14"/>
       <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="14"/>
       <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1493,112 +1572,139 @@
       <c r="K14" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1613,33 +1719,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1657,48 +1736,48 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
@@ -1714,10 +1793,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1742,29 +1821,29 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38">
+      <c r="E6" s="22"/>
+      <c r="F6" s="42">
         <v>44322</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="23" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1783,98 +1862,98 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14"/>
       <c r="F9" s="10">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="14"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="14"/>
       <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="14"/>
       <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1885,13 +1964,13 @@
       <c r="F13" s="10">
         <v>5</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1911,112 +1990,140 @@
       <c r="K14" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -2031,34 +2138,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2075,48 +2154,48 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
@@ -2132,10 +2211,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2160,29 +2239,29 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38">
+      <c r="E6" s="22"/>
+      <c r="F6" s="42">
         <v>44322</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="23" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -2201,98 +2280,98 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14"/>
       <c r="F9" s="10">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="14"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="14"/>
       <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="14"/>
       <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -2303,13 +2382,13 @@
       <c r="F13" s="10">
         <v>5</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -2329,112 +2408,140 @@
       <c r="K14" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -2449,34 +2556,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2493,48 +2572,48 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
@@ -2550,10 +2629,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2578,29 +2657,29 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38">
+      <c r="E6" s="22"/>
+      <c r="F6" s="42">
         <v>44322</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="23" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -2619,92 +2698,92 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14"/>
       <c r="F9" s="10">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="14"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="14"/>
       <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="14"/>
       <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -2713,11 +2792,11 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -2737,112 +2816,140 @@
       <c r="K14" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -2857,22 +2964,372 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571BB059-2B74-4973-8FFA-22C6A17ABFB4}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="36"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="42">
+        <v>44322</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="40"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>3</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="10">
+        <v>3</v>
+      </c>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="10">
+        <v>4</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>2</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>3</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:H20"/>
@@ -2885,372 +3342,22 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:K19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571BB059-2B74-4973-8FFA-22C6A17ABFB4}">
-  <dimension ref="A1:K20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38">
-        <v>44322</v>
-      </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="10">
-        <v>1</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="10">
-        <v>2</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="10">
-        <v>3</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>4</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="10">
-        <v>4</v>
-      </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>2</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>3</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-    </row>
-  </sheetData>
-  <mergeCells count="42">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -3265,34 +3372,423 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945E7267-2BFA-496B-A831-8CAD22B56E6C}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="36"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="22"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="45">
+        <v>44322</v>
+      </c>
+      <c r="G6" s="46"/>
+      <c r="H6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="47"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="F8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>3</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="F11" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="F12" s="10">
+        <v>4</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="28"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="10">
+        <v>5</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="10">
+        <v>6</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="10">
+        <v>7</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="10">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>1</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="27"/>
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>2</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="27"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>3</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>4</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="49">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="I20:K21"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="G9:K9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>